<commit_message>
Revert "Merge branch 'master' into cam"
This reverts commit fd545259e250e893790dca8b27a1cc9fa9737b66.
</commit_message>
<xml_diff>
--- a/docs/Disciplines projet Plan interactif provisoire - v0.xlsx
+++ b/docs/Disciplines projet Plan interactif provisoire - v0.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="21315" windowHeight="10035"/>
+    <workbookView xWindow="1180" yWindow="0" windowWidth="27660" windowHeight="19340"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1976,20 +1981,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E316"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="F160" sqref="F160"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
-    <col min="3" max="3" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="58.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5" customWidth="1"/>
+    <col min="3" max="3" width="38.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.6640625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -2006,7 +2011,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -2023,7 +2028,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -2037,7 +2042,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -2051,7 +2056,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -2065,7 +2070,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -2079,7 +2084,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -2093,7 +2098,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -2107,7 +2112,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -2121,7 +2126,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -2135,7 +2140,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -2149,7 +2154,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -2163,7 +2168,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -2177,7 +2182,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -2191,7 +2196,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -2205,7 +2210,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -2219,7 +2224,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -2233,7 +2238,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -2247,7 +2252,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>40</v>
       </c>
@@ -2261,7 +2266,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -2275,7 +2280,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -2289,7 +2294,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -2303,7 +2308,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -2317,7 +2322,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -2331,7 +2336,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>41</v>
       </c>
@@ -2345,7 +2350,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -2359,7 +2364,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -2373,7 +2378,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -2387,7 +2392,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -2401,7 +2406,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -2415,7 +2420,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -2429,7 +2434,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>41</v>
       </c>
@@ -2443,7 +2448,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -2457,7 +2462,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -2471,7 +2476,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -2485,7 +2490,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -2499,7 +2504,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -2513,7 +2518,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>40</v>
       </c>
@@ -2527,7 +2532,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -2541,7 +2546,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -2555,7 +2560,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -2569,7 +2574,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -2583,7 +2588,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>40</v>
       </c>
@@ -2597,7 +2602,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>40</v>
       </c>
@@ -2611,7 +2616,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>40</v>
       </c>
@@ -2625,7 +2630,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
         <v>40</v>
       </c>
@@ -2639,7 +2644,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
         <v>40</v>
       </c>
@@ -2653,7 +2658,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
         <v>40</v>
       </c>
@@ -2667,7 +2672,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>40</v>
       </c>
@@ -2681,7 +2686,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>40</v>
       </c>
@@ -2695,7 +2700,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
         <v>41</v>
       </c>
@@ -2709,7 +2714,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>41</v>
       </c>
@@ -2723,7 +2728,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>41</v>
       </c>
@@ -2737,7 +2742,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
         <v>41</v>
       </c>
@@ -2751,7 +2756,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
         <v>41</v>
       </c>
@@ -2765,7 +2770,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
         <v>41</v>
       </c>
@@ -2779,7 +2784,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
         <v>41</v>
       </c>
@@ -2793,7 +2798,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
         <v>41</v>
       </c>
@@ -2807,7 +2812,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
         <v>41</v>
       </c>
@@ -2821,7 +2826,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5">
       <c r="A60" t="s">
         <v>41</v>
       </c>
@@ -2835,7 +2840,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5">
       <c r="A61" t="s">
         <v>41</v>
       </c>
@@ -2849,7 +2854,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5">
       <c r="A62" t="s">
         <v>41</v>
       </c>
@@ -2863,7 +2868,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5">
       <c r="A63" t="s">
         <v>41</v>
       </c>
@@ -2877,7 +2882,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5">
       <c r="A64" t="s">
         <v>41</v>
       </c>
@@ -2891,7 +2896,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5">
       <c r="A65" t="s">
         <v>41</v>
       </c>
@@ -2905,7 +2910,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5">
       <c r="A66" t="s">
         <v>41</v>
       </c>
@@ -2919,7 +2924,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5">
       <c r="A67" t="s">
         <v>41</v>
       </c>
@@ -2933,7 +2938,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5">
       <c r="A68" t="s">
         <v>41</v>
       </c>
@@ -2947,7 +2952,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5">
       <c r="A69" t="s">
         <v>41</v>
       </c>
@@ -2961,7 +2966,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5">
       <c r="A70" t="s">
         <v>41</v>
       </c>
@@ -2975,7 +2980,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5">
       <c r="A71" t="s">
         <v>41</v>
       </c>
@@ -2989,7 +2994,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5">
       <c r="A72" t="s">
         <v>41</v>
       </c>
@@ -3003,7 +3008,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5">
       <c r="A73" t="s">
         <v>41</v>
       </c>
@@ -3017,7 +3022,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5">
       <c r="A74" t="s">
         <v>41</v>
       </c>
@@ -3031,7 +3036,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5">
       <c r="A75" t="s">
         <v>41</v>
       </c>
@@ -3045,7 +3050,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5">
       <c r="A76" t="s">
         <v>39</v>
       </c>
@@ -3059,7 +3064,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5">
       <c r="A77" t="s">
         <v>41</v>
       </c>
@@ -3073,7 +3078,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5">
       <c r="A78" t="s">
         <v>41</v>
       </c>
@@ -3087,7 +3092,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5">
       <c r="A79" t="s">
         <v>41</v>
       </c>
@@ -3101,7 +3106,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5">
       <c r="A80" t="s">
         <v>41</v>
       </c>
@@ -3115,7 +3120,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5">
       <c r="A81" t="s">
         <v>41</v>
       </c>
@@ -3129,7 +3134,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5">
       <c r="A82" t="s">
         <v>41</v>
       </c>
@@ -3143,7 +3148,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5">
       <c r="A83" t="s">
         <v>41</v>
       </c>
@@ -3157,7 +3162,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5">
       <c r="A84" t="s">
         <v>41</v>
       </c>
@@ -3171,7 +3176,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5">
       <c r="A85" t="s">
         <v>41</v>
       </c>
@@ -3185,7 +3190,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5">
       <c r="A86" t="s">
         <v>41</v>
       </c>
@@ -3199,7 +3204,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5">
       <c r="A87" t="s">
         <v>41</v>
       </c>
@@ -3213,7 +3218,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5">
       <c r="A88" t="s">
         <v>41</v>
       </c>
@@ -3227,7 +3232,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5">
       <c r="A89" t="s">
         <v>41</v>
       </c>
@@ -3241,7 +3246,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5">
       <c r="A90" t="s">
         <v>41</v>
       </c>
@@ -3255,7 +3260,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5">
       <c r="A91" t="s">
         <v>41</v>
       </c>
@@ -3269,7 +3274,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5">
       <c r="A92" t="s">
         <v>41</v>
       </c>
@@ -3283,7 +3288,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5">
       <c r="A93" t="s">
         <v>41</v>
       </c>
@@ -3297,7 +3302,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5">
       <c r="A94" t="s">
         <v>41</v>
       </c>
@@ -3311,7 +3316,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5">
       <c r="A95" t="s">
         <v>41</v>
       </c>
@@ -3325,7 +3330,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5">
       <c r="A96" t="s">
         <v>41</v>
       </c>
@@ -3339,7 +3344,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5">
       <c r="A97" t="s">
         <v>41</v>
       </c>
@@ -3353,7 +3358,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5">
       <c r="A98" t="s">
         <v>39</v>
       </c>
@@ -3367,7 +3372,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5">
       <c r="A99" t="s">
         <v>40</v>
       </c>
@@ -3381,7 +3386,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5">
       <c r="A100" t="s">
         <v>40</v>
       </c>
@@ -3395,7 +3400,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5">
       <c r="A101" t="s">
         <v>40</v>
       </c>
@@ -3409,7 +3414,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5">
       <c r="A102" t="s">
         <v>40</v>
       </c>
@@ -3423,7 +3428,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5">
       <c r="A103" t="s">
         <v>40</v>
       </c>
@@ -3437,7 +3442,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5">
       <c r="A104" t="s">
         <v>40</v>
       </c>
@@ -3451,7 +3456,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5">
       <c r="A105" t="s">
         <v>40</v>
       </c>
@@ -3465,7 +3470,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5">
       <c r="A106" t="s">
         <v>40</v>
       </c>
@@ -3479,7 +3484,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5">
       <c r="A107" t="s">
         <v>40</v>
       </c>
@@ -3493,7 +3498,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5">
       <c r="A108" t="s">
         <v>40</v>
       </c>
@@ -3507,7 +3512,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5">
       <c r="A109" t="s">
         <v>40</v>
       </c>
@@ -3521,7 +3526,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5">
       <c r="A110" t="s">
         <v>40</v>
       </c>
@@ -3535,7 +3540,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5">
       <c r="A111" t="s">
         <v>40</v>
       </c>
@@ -3549,7 +3554,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5">
       <c r="A112" t="s">
         <v>40</v>
       </c>
@@ -3563,7 +3568,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5">
       <c r="A113" t="s">
         <v>40</v>
       </c>
@@ -3577,7 +3582,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5">
       <c r="A114" t="s">
         <v>40</v>
       </c>
@@ -3591,7 +3596,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5">
       <c r="A115" t="s">
         <v>40</v>
       </c>
@@ -3605,7 +3610,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5">
       <c r="A116" t="s">
         <v>40</v>
       </c>
@@ -3619,7 +3624,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5">
       <c r="A117" t="s">
         <v>40</v>
       </c>
@@ -3633,7 +3638,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5">
       <c r="A118" t="s">
         <v>40</v>
       </c>
@@ -3647,7 +3652,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5">
       <c r="A119" t="s">
         <v>40</v>
       </c>
@@ -3661,7 +3666,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5">
       <c r="A120" t="s">
         <v>40</v>
       </c>
@@ -3675,7 +3680,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5">
       <c r="A121" t="s">
         <v>40</v>
       </c>
@@ -3689,7 +3694,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5">
       <c r="A122" t="s">
         <v>40</v>
       </c>
@@ -3703,7 +3708,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5">
       <c r="A123" t="s">
         <v>40</v>
       </c>
@@ -3717,7 +3722,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5">
       <c r="A124" t="s">
         <v>40</v>
       </c>
@@ -3731,7 +3736,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5">
       <c r="A125" t="s">
         <v>40</v>
       </c>
@@ -3745,7 +3750,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5">
       <c r="A126" t="s">
         <v>36</v>
       </c>
@@ -3759,7 +3764,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5">
       <c r="A127" t="s">
         <v>36</v>
       </c>
@@ -3773,7 +3778,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5">
       <c r="A128" t="s">
         <v>36</v>
       </c>
@@ -3787,7 +3792,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5">
       <c r="A129" t="s">
         <v>36</v>
       </c>
@@ -3801,7 +3806,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5">
       <c r="A130" t="s">
         <v>36</v>
       </c>
@@ -3815,7 +3820,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5">
       <c r="A131" t="s">
         <v>36</v>
       </c>
@@ -3829,7 +3834,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5">
       <c r="A132" t="s">
         <v>36</v>
       </c>
@@ -3843,7 +3848,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5">
       <c r="A133" t="s">
         <v>36</v>
       </c>
@@ -3857,7 +3862,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5">
       <c r="A134" t="s">
         <v>36</v>
       </c>
@@ -3871,7 +3876,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5">
       <c r="A135" t="s">
         <v>36</v>
       </c>
@@ -3885,7 +3890,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5">
       <c r="A136" t="s">
         <v>36</v>
       </c>
@@ -3899,7 +3904,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5">
       <c r="A137" t="s">
         <v>36</v>
       </c>
@@ -3913,7 +3918,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5">
       <c r="A138" t="s">
         <v>36</v>
       </c>
@@ -3927,7 +3932,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5">
       <c r="A139" t="s">
         <v>36</v>
       </c>
@@ -3941,7 +3946,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5">
       <c r="A140" t="s">
         <v>36</v>
       </c>
@@ -3955,7 +3960,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5">
       <c r="A141" t="s">
         <v>36</v>
       </c>
@@ -3969,7 +3974,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5">
       <c r="A142" t="s">
         <v>36</v>
       </c>
@@ -3983,7 +3988,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5">
       <c r="A143" t="s">
         <v>36</v>
       </c>
@@ -3997,7 +4002,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5">
       <c r="A144" t="s">
         <v>36</v>
       </c>
@@ -4011,7 +4016,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5">
       <c r="A145" t="s">
         <v>36</v>
       </c>
@@ -4025,7 +4030,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5">
       <c r="A146" t="s">
         <v>36</v>
       </c>
@@ -4039,7 +4044,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5">
       <c r="A147" t="s">
         <v>36</v>
       </c>
@@ -4053,7 +4058,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5">
       <c r="A148" t="s">
         <v>36</v>
       </c>
@@ -4067,7 +4072,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5">
       <c r="A149" t="s">
         <v>36</v>
       </c>
@@ -4081,7 +4086,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5">
       <c r="A150" t="s">
         <v>36</v>
       </c>
@@ -4095,7 +4100,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5">
       <c r="A151" t="s">
         <v>36</v>
       </c>
@@ -4109,7 +4114,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5">
       <c r="A152" t="s">
         <v>36</v>
       </c>
@@ -4123,7 +4128,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5">
       <c r="A153" t="s">
         <v>36</v>
       </c>
@@ -4137,7 +4142,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5">
       <c r="A154" t="s">
         <v>36</v>
       </c>
@@ -4151,7 +4156,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5">
       <c r="A155" t="s">
         <v>36</v>
       </c>
@@ -4165,7 +4170,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5">
       <c r="A156" t="s">
         <v>36</v>
       </c>
@@ -4179,7 +4184,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5">
       <c r="D157" t="s">
         <v>54</v>
       </c>
@@ -4187,7 +4192,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5">
       <c r="D158" t="s">
         <v>54</v>
       </c>
@@ -4195,7 +4200,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5">
       <c r="D159" t="s">
         <v>54</v>
       </c>
@@ -4203,7 +4208,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5">
       <c r="D160" t="s">
         <v>54</v>
       </c>
@@ -4211,7 +4216,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5">
       <c r="D161" t="s">
         <v>54</v>
       </c>
@@ -4219,7 +4224,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5">
       <c r="D162" t="s">
         <v>54</v>
       </c>
@@ -4227,7 +4232,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5">
       <c r="D163" t="s">
         <v>54</v>
       </c>
@@ -4235,7 +4240,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5">
       <c r="A164" t="s">
         <v>36</v>
       </c>
@@ -4249,7 +4254,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5">
       <c r="A165" t="s">
         <v>36</v>
       </c>
@@ -4263,7 +4268,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5">
       <c r="A166" t="s">
         <v>36</v>
       </c>
@@ -4277,7 +4282,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5">
       <c r="A167" t="s">
         <v>36</v>
       </c>
@@ -4291,7 +4296,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5">
       <c r="A168" t="s">
         <v>36</v>
       </c>
@@ -4305,7 +4310,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5">
       <c r="A169" t="s">
         <v>36</v>
       </c>
@@ -4319,7 +4324,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5">
       <c r="A170" t="s">
         <v>36</v>
       </c>
@@ -4333,7 +4338,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5">
       <c r="D171" t="s">
         <v>53</v>
       </c>
@@ -4341,7 +4346,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5">
       <c r="D172" t="s">
         <v>53</v>
       </c>
@@ -4349,7 +4354,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5">
       <c r="D173" t="s">
         <v>53</v>
       </c>
@@ -4357,7 +4362,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5">
       <c r="D174" t="s">
         <v>53</v>
       </c>
@@ -4365,7 +4370,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5">
       <c r="D175" t="s">
         <v>53</v>
       </c>
@@ -4373,7 +4378,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5">
       <c r="D176" t="s">
         <v>53</v>
       </c>
@@ -4381,7 +4386,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5">
       <c r="D177" t="s">
         <v>53</v>
       </c>
@@ -4389,7 +4394,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5">
       <c r="A178" t="s">
         <v>36</v>
       </c>
@@ -4403,7 +4408,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5">
       <c r="A179" t="s">
         <v>36</v>
       </c>
@@ -4417,7 +4422,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5">
       <c r="A180" t="s">
         <v>36</v>
       </c>
@@ -4431,7 +4436,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5">
       <c r="D181" t="s">
         <v>64</v>
       </c>
@@ -4439,7 +4444,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5">
       <c r="D182" t="s">
         <v>64</v>
       </c>
@@ -4447,7 +4452,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5">
       <c r="D183" t="s">
         <v>64</v>
       </c>
@@ -4455,7 +4460,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5">
       <c r="D184" t="s">
         <v>64</v>
       </c>
@@ -4463,7 +4468,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5">
       <c r="D185" t="s">
         <v>64</v>
       </c>
@@ -4471,7 +4476,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5">
       <c r="D186" t="s">
         <v>64</v>
       </c>
@@ -4479,7 +4484,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5">
       <c r="D187" t="s">
         <v>64</v>
       </c>
@@ -4487,7 +4492,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5">
       <c r="A188" t="s">
         <v>36</v>
       </c>
@@ -4501,7 +4506,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5">
       <c r="A189" t="s">
         <v>36</v>
       </c>
@@ -4515,7 +4520,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5">
       <c r="A190" t="s">
         <v>36</v>
       </c>
@@ -4529,7 +4534,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5">
       <c r="A191" t="s">
         <v>36</v>
       </c>
@@ -4543,7 +4548,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5">
       <c r="A192" t="s">
         <v>36</v>
       </c>
@@ -4557,7 +4562,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5">
       <c r="A193" t="s">
         <v>36</v>
       </c>
@@ -4571,7 +4576,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5">
       <c r="A194" t="s">
         <v>36</v>
       </c>
@@ -4585,7 +4590,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5">
       <c r="A195" t="s">
         <v>36</v>
       </c>
@@ -4599,7 +4604,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5">
       <c r="A196" t="s">
         <v>36</v>
       </c>
@@ -4613,7 +4618,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5">
       <c r="A197" t="s">
         <v>36</v>
       </c>
@@ -4627,7 +4632,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5">
       <c r="A198" t="s">
         <v>36</v>
       </c>
@@ -4641,7 +4646,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5">
       <c r="A199" t="s">
         <v>36</v>
       </c>
@@ -4655,7 +4660,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5">
       <c r="A200" t="s">
         <v>36</v>
       </c>
@@ -4669,7 +4674,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5">
       <c r="D201" t="s">
         <v>71</v>
       </c>
@@ -4677,7 +4682,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5">
       <c r="D202" t="s">
         <v>71</v>
       </c>
@@ -4685,7 +4690,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5">
       <c r="D203" t="s">
         <v>71</v>
       </c>
@@ -4693,7 +4698,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5">
       <c r="D204" t="s">
         <v>71</v>
       </c>
@@ -4701,7 +4706,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5">
       <c r="D205" t="s">
         <v>71</v>
       </c>
@@ -4709,7 +4714,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5">
       <c r="D206" t="s">
         <v>71</v>
       </c>
@@ -4717,7 +4722,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5">
       <c r="D207" t="s">
         <v>71</v>
       </c>
@@ -4725,7 +4730,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5">
       <c r="A208" t="s">
         <v>36</v>
       </c>
@@ -4739,7 +4744,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5">
       <c r="A209" t="s">
         <v>36</v>
       </c>
@@ -4753,7 +4758,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5">
       <c r="A210" t="s">
         <v>36</v>
       </c>
@@ -4767,7 +4772,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5">
       <c r="A211" t="s">
         <v>36</v>
       </c>
@@ -4781,7 +4786,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5">
       <c r="A212" t="s">
         <v>36</v>
       </c>
@@ -4795,7 +4800,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5">
       <c r="A213" t="s">
         <v>36</v>
       </c>
@@ -4809,7 +4814,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5">
       <c r="A214" t="s">
         <v>36</v>
       </c>
@@ -4823,7 +4828,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5">
       <c r="A215" t="s">
         <v>36</v>
       </c>
@@ -4837,7 +4842,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5">
       <c r="A216" t="s">
         <v>36</v>
       </c>
@@ -4851,7 +4856,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5">
       <c r="A217" t="s">
         <v>36</v>
       </c>
@@ -4865,7 +4870,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5">
       <c r="A218" t="s">
         <v>36</v>
       </c>
@@ -4879,7 +4884,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5">
       <c r="A219" t="s">
         <v>36</v>
       </c>
@@ -4893,7 +4898,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5">
       <c r="A220" t="s">
         <v>36</v>
       </c>
@@ -4907,7 +4912,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5">
       <c r="A221" t="s">
         <v>36</v>
       </c>
@@ -4921,7 +4926,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5">
       <c r="A222" t="s">
         <v>36</v>
       </c>
@@ -4935,7 +4940,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5">
       <c r="A223" t="s">
         <v>36</v>
       </c>
@@ -4949,7 +4954,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5">
       <c r="A224" t="s">
         <v>36</v>
       </c>
@@ -4963,7 +4968,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5">
       <c r="A225" t="s">
         <v>36</v>
       </c>
@@ -4977,7 +4982,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5">
       <c r="A226" t="s">
         <v>40</v>
       </c>
@@ -4991,7 +4996,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5">
       <c r="A227" t="s">
         <v>40</v>
       </c>
@@ -5005,7 +5010,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5">
       <c r="A228" t="s">
         <v>40</v>
       </c>
@@ -5019,7 +5024,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5">
       <c r="A229" t="s">
         <v>40</v>
       </c>
@@ -5033,7 +5038,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5">
       <c r="A230" t="s">
         <v>40</v>
       </c>
@@ -5047,7 +5052,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5">
       <c r="A231" t="s">
         <v>40</v>
       </c>
@@ -5061,7 +5066,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5">
       <c r="A232" t="s">
         <v>40</v>
       </c>
@@ -5075,7 +5080,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5">
       <c r="A233" t="s">
         <v>40</v>
       </c>
@@ -5089,7 +5094,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5">
       <c r="A234" t="s">
         <v>40</v>
       </c>
@@ -5103,7 +5108,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5">
       <c r="A235" t="s">
         <v>40</v>
       </c>
@@ -5117,7 +5122,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5">
       <c r="A236" t="s">
         <v>40</v>
       </c>
@@ -5131,7 +5136,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5">
       <c r="A237" t="s">
         <v>40</v>
       </c>
@@ -5145,7 +5150,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5">
       <c r="A238" t="s">
         <v>40</v>
       </c>
@@ -5159,7 +5164,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5">
       <c r="A239" t="s">
         <v>40</v>
       </c>
@@ -5173,7 +5178,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5">
       <c r="A240" t="s">
         <v>40</v>
       </c>
@@ -5187,7 +5192,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5">
       <c r="A241" t="s">
         <v>40</v>
       </c>
@@ -5201,7 +5206,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5">
       <c r="A242" t="s">
         <v>40</v>
       </c>
@@ -5215,7 +5220,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5">
       <c r="A243" t="s">
         <v>40</v>
       </c>
@@ -5229,7 +5234,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5">
       <c r="A244" t="s">
         <v>40</v>
       </c>
@@ -5243,7 +5248,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5">
       <c r="A245" t="s">
         <v>40</v>
       </c>
@@ -5257,7 +5262,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5">
       <c r="A246" t="s">
         <v>40</v>
       </c>
@@ -5271,7 +5276,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5">
       <c r="A247" t="s">
         <v>40</v>
       </c>
@@ -5285,7 +5290,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5">
       <c r="A248" t="s">
         <v>40</v>
       </c>
@@ -5299,7 +5304,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5">
       <c r="A249" t="s">
         <v>40</v>
       </c>
@@ -5313,7 +5318,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5">
       <c r="A250" t="s">
         <v>40</v>
       </c>
@@ -5327,7 +5332,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5">
       <c r="A251" t="s">
         <v>40</v>
       </c>
@@ -5341,7 +5346,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5">
       <c r="A252" t="s">
         <v>40</v>
       </c>
@@ -5355,7 +5360,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5">
       <c r="A253" t="s">
         <v>40</v>
       </c>
@@ -5369,7 +5374,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5">
       <c r="A254" t="s">
         <v>40</v>
       </c>
@@ -5383,7 +5388,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5">
       <c r="A255" t="s">
         <v>40</v>
       </c>
@@ -5397,7 +5402,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5">
       <c r="A256" t="s">
         <v>40</v>
       </c>
@@ -5411,7 +5416,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5">
       <c r="A257" t="s">
         <v>40</v>
       </c>
@@ -5425,7 +5430,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5">
       <c r="A258" t="s">
         <v>40</v>
       </c>
@@ -5439,7 +5444,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5">
       <c r="A259" t="s">
         <v>40</v>
       </c>
@@ -5453,7 +5458,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5">
       <c r="A260" t="s">
         <v>40</v>
       </c>
@@ -5467,7 +5472,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5">
       <c r="A261" t="s">
         <v>40</v>
       </c>
@@ -5481,7 +5486,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5">
       <c r="A262" t="s">
         <v>40</v>
       </c>
@@ -5495,7 +5500,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5">
       <c r="A263" t="s">
         <v>40</v>
       </c>
@@ -5509,7 +5514,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5">
       <c r="A264" t="s">
         <v>40</v>
       </c>
@@ -5523,7 +5528,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5">
       <c r="A265" t="s">
         <v>40</v>
       </c>
@@ -5537,7 +5542,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5">
       <c r="A266" t="s">
         <v>40</v>
       </c>
@@ -5551,7 +5556,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5">
       <c r="A267" t="s">
         <v>40</v>
       </c>
@@ -5565,7 +5570,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5">
       <c r="A268" t="s">
         <v>40</v>
       </c>
@@ -5579,7 +5584,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5">
       <c r="A269" t="s">
         <v>40</v>
       </c>
@@ -5593,7 +5598,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5">
       <c r="A270" t="s">
         <v>40</v>
       </c>
@@ -5607,7 +5612,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5">
       <c r="A271" t="s">
         <v>37</v>
       </c>
@@ -5621,7 +5626,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:5">
       <c r="A272" t="s">
         <v>38</v>
       </c>
@@ -5635,7 +5640,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:5">
       <c r="A273" t="s">
         <v>38</v>
       </c>
@@ -5649,7 +5654,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5">
       <c r="A274" t="s">
         <v>38</v>
       </c>
@@ -5663,7 +5668,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5">
       <c r="A275" t="s">
         <v>38</v>
       </c>
@@ -5677,7 +5682,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:5">
       <c r="A276" t="s">
         <v>38</v>
       </c>
@@ -5691,7 +5696,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5">
       <c r="A277" t="s">
         <v>38</v>
       </c>
@@ -5705,7 +5710,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5">
       <c r="A278" t="s">
         <v>38</v>
       </c>
@@ -5719,7 +5724,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:5">
       <c r="A279" t="s">
         <v>38</v>
       </c>
@@ -5733,7 +5738,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:5">
       <c r="A280" t="s">
         <v>38</v>
       </c>
@@ -5747,7 +5752,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:5">
       <c r="A281" t="s">
         <v>38</v>
       </c>
@@ -5761,7 +5766,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:5">
       <c r="A282" t="s">
         <v>38</v>
       </c>
@@ -5775,7 +5780,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:5">
       <c r="A283" t="s">
         <v>38</v>
       </c>
@@ -5789,7 +5794,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5">
       <c r="A284" t="s">
         <v>38</v>
       </c>
@@ -5803,7 +5808,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:5">
       <c r="A285" t="s">
         <v>38</v>
       </c>
@@ -5817,7 +5822,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:5">
       <c r="A286" t="s">
         <v>38</v>
       </c>
@@ -5831,7 +5836,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:5">
       <c r="A287" t="s">
         <v>38</v>
       </c>
@@ -5845,7 +5850,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:5">
       <c r="A288" t="s">
         <v>38</v>
       </c>
@@ -5859,7 +5864,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5">
       <c r="A289" t="s">
         <v>38</v>
       </c>
@@ -5873,7 +5878,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:5">
       <c r="A290" t="s">
         <v>38</v>
       </c>
@@ -5887,7 +5892,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5">
       <c r="A291" t="s">
         <v>38</v>
       </c>
@@ -5901,7 +5906,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:5">
       <c r="A292" t="s">
         <v>38</v>
       </c>
@@ -5915,7 +5920,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:5">
       <c r="A293" t="s">
         <v>38</v>
       </c>
@@ -5929,7 +5934,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:5">
       <c r="A294" t="s">
         <v>38</v>
       </c>
@@ -5943,7 +5948,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:5">
       <c r="A295" t="s">
         <v>38</v>
       </c>
@@ -5957,7 +5962,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5">
       <c r="A296" t="s">
         <v>38</v>
       </c>
@@ -5971,7 +5976,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5">
       <c r="A297" t="s">
         <v>38</v>
       </c>
@@ -5985,7 +5990,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:5">
       <c r="A298" t="s">
         <v>38</v>
       </c>
@@ -5999,7 +6004,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:5">
       <c r="A299" t="s">
         <v>38</v>
       </c>
@@ -6013,7 +6018,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:5">
       <c r="A300" t="s">
         <v>38</v>
       </c>
@@ -6027,7 +6032,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:5">
       <c r="A301" t="s">
         <v>38</v>
       </c>
@@ -6041,7 +6046,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:5">
       <c r="A302" t="s">
         <v>39</v>
       </c>
@@ -6055,7 +6060,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:5">
       <c r="A303" t="s">
         <v>39</v>
       </c>
@@ -6069,7 +6074,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:5">
       <c r="A304" t="s">
         <v>39</v>
       </c>
@@ -6083,7 +6088,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:5">
       <c r="A305" t="s">
         <v>39</v>
       </c>
@@ -6097,7 +6102,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:5">
       <c r="A306" t="s">
         <v>39</v>
       </c>
@@ -6111,7 +6116,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:5">
       <c r="A307" t="s">
         <v>39</v>
       </c>
@@ -6125,7 +6130,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:5">
       <c r="A308" t="s">
         <v>39</v>
       </c>
@@ -6139,7 +6144,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:5">
       <c r="A309" t="s">
         <v>39</v>
       </c>
@@ -6153,7 +6158,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:5">
       <c r="A310" t="s">
         <v>39</v>
       </c>
@@ -6167,7 +6172,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:5">
       <c r="A311" t="s">
         <v>39</v>
       </c>
@@ -6181,7 +6186,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:5">
       <c r="A312" t="s">
         <v>39</v>
       </c>
@@ -6195,7 +6200,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:5">
       <c r="A313" t="s">
         <v>39</v>
       </c>
@@ -6209,7 +6214,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:5">
       <c r="A314" t="s">
         <v>39</v>
       </c>
@@ -6223,7 +6228,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:5">
       <c r="A315" t="s">
         <v>39</v>
       </c>
@@ -6237,7 +6242,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:5">
       <c r="A316" t="s">
         <v>39</v>
       </c>
@@ -6253,7 +6258,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6263,9 +6273,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6275,8 +6290,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>